<commit_message>
new rubric, fixed errors in other
</commit_message>
<xml_diff>
--- a/Labs/Lab5/Assignment5Rubric.xlsx
+++ b/Labs/Lab5/Assignment5Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Repos\CS246-CourseMaterials\Labs\Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADB09F4-39FE-406E-A5BE-108A8ABD1FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D61325-0DA4-4995-BF98-4D7D263BBD6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="495" windowWidth="10620" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="14760" yWindow="495" windowWidth="10620" windowHeight="14640" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Requirements</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>CS246 Assignment 2 Rubric</t>
-  </si>
-  <si>
-    <t>Agile project management</t>
   </si>
   <si>
     <t>CS246 Assignment 5 Rubric</t>
@@ -477,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -488,14 +482,14 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,13 +507,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -527,7 +521,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -535,7 +529,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -543,7 +537,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>20</v>
@@ -551,7 +545,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>5</v>
@@ -559,7 +553,7 @@
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -567,7 +561,7 @@
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
         <f>SUM(B6:B11)</f>
@@ -580,7 +574,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
     </row>
@@ -598,7 +592,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
         <f>SUM(B15:B17)</f>
@@ -624,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -657,20 +651,20 @@
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -681,7 +675,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -692,7 +686,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -703,7 +697,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>20</v>
@@ -714,7 +708,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>5</v>
@@ -725,7 +719,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -754,7 +748,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -776,7 +770,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
         <f>SUM(B15:B17)</f>
@@ -802,5 +796,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>